<commit_message>
passed ellipticity angular limits to degrees
</commit_message>
<xml_diff>
--- a/cell_tracker/data/excel_trajs_example.xlsx
+++ b/cell_tracker/data/excel_trajs_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuill1" sheetId="1" state="visible" r:id="rId2"/>
@@ -66,13 +66,13 @@
     <t>FileName</t>
   </si>
   <si>
-    <t>20130724-NLSDsRedUbCadhGFP-S1-NLSDsRed_T0.tif</t>
+    <t>test_cell.tif</t>
   </si>
   <si>
     <t>SizeT</t>
   </si>
   <si>
-    <t>(32,)</t>
+    <t>32</t>
   </si>
   <si>
     <t>TimeIncrement</t>
@@ -206,10 +206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A17" activeCellId="0" pane="topLeft" sqref="A17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F2" activeCellId="0" pane="topLeft" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -238,7 +238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -255,10 +255,11 @@
         <v>14.8213473085478</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+        <f aca="false">A2*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="1" t="n">
         <v>0</v>
       </c>
@@ -275,10 +276,11 @@
         <v>10.2180636041147</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+        <f aca="false">A3*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="1" t="n">
         <v>0</v>
       </c>
@@ -295,10 +297,11 @@
         <v>10.8379048540859</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+        <f aca="false">A4*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
@@ -315,10 +318,11 @@
         <v>11.0006836475529</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+        <f aca="false">A5*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="1" t="n">
         <v>0</v>
       </c>
@@ -335,10 +339,11 @@
         <v>19.4556294265094</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+        <f aca="false">A6*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="1" t="n">
         <v>1</v>
       </c>
@@ -355,10 +360,11 @@
         <v>16.8589404408339</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+        <f aca="false">A7*3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="A8" s="1" t="n">
         <v>1</v>
       </c>
@@ -375,10 +381,11 @@
         <v>9.92675196343249</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+        <f aca="false">A8*3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="1" t="n">
         <v>1</v>
       </c>
@@ -395,10 +402,11 @@
         <v>9.69337422490041</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+        <f aca="false">A9*3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="1" t="n">
         <v>1</v>
       </c>
@@ -415,10 +423,11 @@
         <v>11.3861600962334</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
+        <f aca="false">A10*3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="A11" s="1" t="n">
         <v>1</v>
       </c>
@@ -435,10 +444,11 @@
         <v>19.9656922967087</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+        <f aca="false">A11*3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="1" t="n">
         <v>2</v>
       </c>
@@ -455,10 +465,11 @@
         <v>15.5992011921228</v>
       </c>
       <c r="F12" s="0" t="n">
+        <f aca="false">A12*3</f>
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="A13" s="1" t="n">
         <v>2</v>
       </c>
@@ -475,10 +486,11 @@
         <v>9.57676564415248</v>
       </c>
       <c r="F13" s="0" t="n">
+        <f aca="false">A13*3</f>
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
       <c r="A14" s="1" t="n">
         <v>2</v>
       </c>
@@ -495,10 +507,11 @@
         <v>9.86534139498968</v>
       </c>
       <c r="F14" s="0" t="n">
+        <f aca="false">A14*3</f>
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="A15" s="1" t="n">
         <v>2</v>
       </c>
@@ -515,10 +528,11 @@
         <v>11.34183596941</v>
       </c>
       <c r="F15" s="0" t="n">
+        <f aca="false">A15*3</f>
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="A16" s="1" t="n">
         <v>2</v>
       </c>
@@ -535,7 +549,533 @@
         <v>19.0796118638354</v>
       </c>
       <c r="F16" s="0" t="n">
+        <f aca="false">A16*3</f>
         <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>32.9964454435101</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>35.2666953810235</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>15.8213473085478</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">A17*3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>19.5240412189556</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>36.309109638789</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>11.2180636041147</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">A18*3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>19.0908132781387</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>30.2342857858429</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>11.8379048540859</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">A19*3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>23.7555488359548</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>40.1811103967966</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>12.0006836475529</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">A20*3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>28.2873142006715</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>34.8355605231413</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>20.4556294265094</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">A21*3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>33.3325923436185</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>34.1440455393686</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>17.8589404408339</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">A22*3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>20.7295485145007</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>36.346118674086</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>10.9267519634325</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">A23*3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>20.7393571042163</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>30.4828718760724</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>10.6933742249004</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">A24*3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>25.1722501260339</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>40.5229243552995</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>12.3861600962334</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">A25*3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>27.2248519198799</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>35.073547388802</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>20.9656922967087</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">A26*3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>32.7385278608004</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>33.537971601179</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>16.5992011921228</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">A27*3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>20.2531530895127</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>35.9615405291482</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>10.5767656441525</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">A28*3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>20.8893388991168</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>30.7067599409612</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>10.8653413949897</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">A29*3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>25.6716894653534</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>40.7764759689777</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>12.34183596941</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">A30*3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>26.0118314228904</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>34.6022850197921</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>20.0796118638354</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">A31*3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
+      <c r="A32" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>33.9964454435101</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>36.2666953810235</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>16.8213473085478</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">A32*3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>20.5240412189556</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>37.309109638789</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>12.2180636041147</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <f aca="false">A33*3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>20.0908132781387</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>31.2342857858429</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>12.8379048540859</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">A34*3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>24.7555488359548</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>41.1811103967966</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>13.0006836475529</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">A35*3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>29.2873142006715</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>35.8355605231413</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>21.4556294265094</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">A36*3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>34.3325923436185</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>35.1440455393686</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>18.8589404408339</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <f aca="false">A37*3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>21.7295485145007</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>37.346118674086</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>11.9267519634325</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <f aca="false">A38*3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
+      <c r="A39" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>21.7393571042163</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>31.4828718760724</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>11.6933742249004</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">A39*3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="40">
+      <c r="A40" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>26.1722501260339</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>41.5229243552995</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>13.3861600962334</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">A40*3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
+      <c r="A41" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>28.2248519198799</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>36.073547388802</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>21.9656922967087</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">A41*3</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -556,8 +1096,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>